<commit_message>
Continued work on excel calculations
</commit_message>
<xml_diff>
--- a/measurements/20130516_transformation/Koordinatentransformation.xlsx
+++ b/measurements/20130516_transformation/Koordinatentransformation.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="28455" windowHeight="13290" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="28455" windowHeight="13290" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Messaufbau_Messdaten" sheetId="1" r:id="rId1"/>
     <sheet name="Modell+Rechnung" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="testing_ground" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="d_10">Messaufbau_Messdaten!$I$9</definedName>
     <definedName name="d_20">Messaufbau_Messdaten!$I$10</definedName>
     <definedName name="d_30">Messaufbau_Messdaten!$I$11</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>(0,0)</t>
   </si>
@@ -118,13 +117,22 @@
   </si>
   <si>
     <t>d_30</t>
+  </si>
+  <si>
+    <t>x_1</t>
+  </si>
+  <si>
+    <t>x_2</t>
+  </si>
+  <si>
+    <t>x_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +155,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -245,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -265,6 +279,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1523,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1603,12 +1618,344 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B4:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:L37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="2:10">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>-5</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9">
+        <f>MDETERM(B4:D6)</f>
+        <v>113.99999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11">
+        <f>$H4</f>
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <f>C4</f>
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <f>D4</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12">
+        <f>$H5</f>
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <f>C5</f>
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <f>D5</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13">
+        <f>$H6</f>
+        <v>-3</v>
+      </c>
+      <c r="C13">
+        <f>C6</f>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <f>D6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15">
+        <f>B16/$B$9</f>
+        <v>15.754385964912286</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16">
+        <f>MDETERM(B11:D13)</f>
+        <v>1796.0000000000002</v>
+      </c>
+      <c r="H16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16">
+        <f>B23/$B$9</f>
+        <v>-8.2894736842105292</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="H17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17">
+        <f>B30/$B$9</f>
+        <v>0.14912280701754368</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18">
+        <f>B4</f>
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <f>$H4</f>
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <f>D4</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="B19">
+        <f>B5</f>
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <f>$H5</f>
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <f>D5</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20">
+        <f>B6</f>
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <f>$H6</f>
+        <v>-3</v>
+      </c>
+      <c r="D20">
+        <f>D6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="H21">
+        <f>MMULT(B4:D4,$J$15:$J$17)</f>
+        <v>15.000000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="H22">
+        <f t="shared" ref="H22:H23" si="0">MMULT(B5:D5,$J$15:$J$17)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="B23">
+        <f>MDETERM(B18:D20)</f>
+        <v>-945</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>-3.0000000000000018</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25">
+        <f>B4</f>
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <f>C4</f>
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <f>$H4</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26">
+        <f t="shared" ref="B26:C26" si="1">B5</f>
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:D27" si="2">$H5</f>
+        <v>20</v>
+      </c>
+      <c r="H26">
+        <f>MMULT(MINVERSE(B4:D6),H4:H6)</f>
+        <v>15.754385964912284</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27">
+        <f t="shared" ref="B27:C27" si="3">B6</f>
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30">
+        <f>MDETERM(B25:D27)</f>
+        <v>16.999999999999975</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="H32" s="17">
+        <f>INDEX(MINVERSE($B$4:$D$6),ROW(A1),COLUMN(A1))</f>
+        <v>0.47368421052631582</v>
+      </c>
+      <c r="I32" s="17">
+        <f t="shared" ref="I32:J32" si="4">INDEX(MINVERSE($B$4:$D$6),ROW(B1),COLUMN(B1))</f>
+        <v>0.35087719298245623</v>
+      </c>
+      <c r="J32" s="17">
+        <f t="shared" si="4"/>
+        <v>-0.54385964912280715</v>
+      </c>
+      <c r="L32">
+        <f>MMULT($H$32:$J$34,$H$4:$H$6)</f>
+        <v>15.754385964912284</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="B33">
+        <f>MINVERSE(B4:D6)</f>
+        <v>0.47368421052631582</v>
+      </c>
+      <c r="H33" s="17">
+        <f t="shared" ref="H33:H34" si="5">INDEX(MINVERSE($B$4:$D$6),ROW(A2),COLUMN(A2))</f>
+        <v>-0.26315789473684215</v>
+      </c>
+      <c r="I33" s="17">
+        <f t="shared" ref="I33:I34" si="6">INDEX(MINVERSE($B$4:$D$6),ROW(B2),COLUMN(B2))</f>
+        <v>-0.15789473684210528</v>
+      </c>
+      <c r="J33" s="17">
+        <f t="shared" ref="J33:J34" si="7">INDEX(MINVERSE($B$4:$D$6),ROW(C2),COLUMN(C2))</f>
+        <v>0.39473684210526322</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ref="L33:L34" si="8">MMULT($H$32:$J$34,$H$4:$H$6)</f>
+        <v>15.754385964912284</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="H34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="I34" s="17">
+        <f t="shared" si="6"/>
+        <v>-7.0175438596491238E-2</v>
+      </c>
+      <c r="J34" s="17">
+        <f t="shared" si="7"/>
+        <v>8.7719298245614134E-3</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="8"/>
+        <v>15.754385964912284</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12">
+      <c r="B35" s="17">
+        <f>INDEX(MMULT(MINVERSE($B$4:$D$6),$H$4:$H$6),ROW(A1),COLUMN(A1))</f>
+        <v>15.754385964912284</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36" s="17">
+        <f t="shared" ref="B36:D36" si="9">INDEX(MMULT(MINVERSE($B$4:$D$6),$H$4:$H$6),ROW(A2),COLUMN(A2))</f>
+        <v>-8.2894736842105274</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+    </row>
+    <row r="37" spans="2:12">
+      <c r="B37" s="17">
+        <f t="shared" ref="B37:D37" si="10">INDEX(MMULT(MINVERSE($B$4:$D$6),$H$4:$H$6),ROW(A3),COLUMN(A3))</f>
+        <v>0.14912280701754371</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>